<commit_message>
alteração em lon sdi
</commit_message>
<xml_diff>
--- a/static/resources/KM MGA SDI.xlsx
+++ b/static/resources/KM MGA SDI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\0338138\Desktop\kmweb2\onde_a_linha_desligou_web\static\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\0338138\Desktop\kmteste\onde_a_linha_desligou_web_debug\static\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5415F2B7-A44A-4657-B838-EB6641EAA2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C716B3BB-0784-4022-908A-3CACB4DDBFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="120">
   <si>
     <t>CODIGO</t>
   </si>
@@ -54,18 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">MARIALVA                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANDAGUARI                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SABAUDIA                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARAPONGAS                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLANDIA                                </t>
   </si>
   <si>
     <t>SETOR</t>
@@ -842,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE1B1B9-790A-43C6-AAB7-E729AE3660EF}">
-  <dimension ref="A1:R174"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53:G174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,44 +844,44 @@
   <sheetData>
     <row r="1" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -902,22 +890,22 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>0.111</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -933,10 +921,10 @@
         <v>0.1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N2" s="6">
         <v>17.3</v>
@@ -948,22 +936,22 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3">
         <v>0.108</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -979,10 +967,10 @@
         <v>0.2</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N3" s="6">
         <v>17.2</v>
@@ -994,22 +982,22 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>0.36909999999999998</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -1025,10 +1013,10 @@
         <v>0.6</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N4" s="6">
         <v>16.8</v>
@@ -1040,22 +1028,22 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>0.3548</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -1071,10 +1059,10 @@
         <v>0.9</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="N5" s="6">
         <v>16.5</v>
@@ -1086,22 +1074,22 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3">
         <v>0.30009999999999998</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
@@ -1117,10 +1105,10 @@
         <v>1.2</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N6" s="6">
         <v>16.2</v>
@@ -1132,22 +1120,22 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3">
         <v>0.28460000000000002</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
@@ -1163,10 +1151,10 @@
         <v>1.5</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N7" s="6">
         <v>15.9</v>
@@ -1180,22 +1168,22 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3">
         <v>0.6048</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>3</v>
@@ -1211,10 +1199,10 @@
         <v>2.1</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N8" s="6">
         <v>15.3</v>
@@ -1226,22 +1214,22 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3">
         <v>0.3649</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
@@ -1257,10 +1245,10 @@
         <v>2.5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="N9" s="6">
         <v>14.9</v>
@@ -1272,22 +1260,22 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3">
         <v>0.36530000000000001</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -1303,10 +1291,10 @@
         <v>2.9</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N10" s="6">
         <v>14.6</v>
@@ -1318,22 +1306,22 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3">
         <v>0.34989999999999999</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>3</v>
@@ -1349,10 +1337,10 @@
         <v>3.2</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N11" s="6">
         <v>14.2</v>
@@ -1364,22 +1352,22 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
         <v>0.37990000000000002</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
         <v>3</v>
@@ -1395,10 +1383,10 @@
         <v>3.6</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N12" s="6">
         <v>13.8</v>
@@ -1410,22 +1398,22 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3">
         <v>0.44500000000000001</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
         <v>3</v>
@@ -1441,10 +1429,10 @@
         <v>4</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N13" s="6">
         <v>13.4</v>
@@ -1456,22 +1444,22 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>0.32540000000000002</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s">
         <v>3</v>
@@ -1487,10 +1475,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="N14" s="6">
         <v>13.1</v>
@@ -1502,22 +1490,22 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>0.34510000000000002</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
         <v>3</v>
@@ -1533,10 +1521,10 @@
         <v>4.7</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="N15" s="6">
         <v>12.7</v>
@@ -1548,22 +1536,22 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
         <v>0.40439999999999998</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G16" t="s">
         <v>3</v>
@@ -1579,10 +1567,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N16" s="6">
         <v>12.3</v>
@@ -1594,22 +1582,22 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>0.36480000000000001</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
         <v>3</v>
@@ -1625,10 +1613,10 @@
         <v>5.5</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N17" s="6">
         <v>11.9</v>
@@ -1640,22 +1628,22 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B18" s="3">
         <v>0.55569999999999997</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
         <v>3</v>
@@ -1671,10 +1659,10 @@
         <v>6</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N18" s="6">
         <v>11.4</v>
@@ -1686,22 +1674,22 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
         <v>0.23480000000000001</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
         <v>3</v>
@@ -1717,10 +1705,10 @@
         <v>6.3</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="N19" s="6">
         <v>11.1</v>
@@ -1732,22 +1720,22 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3">
         <v>0.29980000000000001</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
         <v>3</v>
@@ -1763,10 +1751,10 @@
         <v>6.6</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N20" s="6">
         <v>10.8</v>
@@ -1778,22 +1766,22 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B21" s="3">
         <v>0.32519999999999999</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G21" t="s">
         <v>3</v>
@@ -1809,10 +1797,10 @@
         <v>6.9</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N21" s="6">
         <v>10.5</v>
@@ -1824,22 +1812,22 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B22" s="3">
         <v>0.39560000000000001</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G22" t="s">
         <v>3</v>
@@ -1855,10 +1843,10 @@
         <v>7.3</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N22" s="6">
         <v>10.1</v>
@@ -1870,22 +1858,22 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B23" s="3">
         <v>0.315</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G23" t="s">
         <v>3</v>
@@ -1901,10 +1889,10 @@
         <v>7.6</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N23" s="6">
         <v>9.8000000000000007</v>
@@ -1916,22 +1904,22 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24" s="3">
         <v>0.30059999999999998</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G24" t="s">
         <v>3</v>
@@ -1947,10 +1935,10 @@
         <v>7.9</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N24" s="6">
         <v>9.5</v>
@@ -1962,22 +1950,22 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B25" s="3">
         <v>0.3483</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G25" t="s">
         <v>3</v>
@@ -1993,10 +1981,10 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N25" s="6">
         <v>9.1999999999999993</v>
@@ -2008,22 +1996,22 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B26" s="3">
         <v>0.61480000000000001</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G26" t="s">
         <v>3</v>
@@ -2039,10 +2027,10 @@
         <v>8.9</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N26" s="6">
         <v>8.5</v>
@@ -2054,22 +2042,22 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B27" s="3">
         <v>0.40500000000000003</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
@@ -2085,10 +2073,10 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="N27" s="6">
         <v>8.1</v>
@@ -2100,22 +2088,22 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B28" s="3">
         <v>0.42030000000000001</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
@@ -2131,10 +2119,10 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="N28" s="6">
         <v>7.7</v>
@@ -2146,22 +2134,22 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B29" s="3">
         <v>0.42520000000000002</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
@@ -2177,10 +2165,10 @@
         <v>10.1</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N29" s="6">
         <v>7.3</v>
@@ -2192,22 +2180,22 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B30" s="3">
         <v>0.43980000000000002</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
@@ -2223,10 +2211,10 @@
         <v>10.6</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N30" s="6">
         <v>6.9</v>
@@ -2238,22 +2226,22 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B31" s="3">
         <v>0.4002</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
@@ -2269,10 +2257,10 @@
         <v>11</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N31" s="6">
         <v>6.5</v>
@@ -2284,22 +2272,22 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B32" s="3">
         <v>0.36470000000000002</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
@@ -2315,10 +2303,10 @@
         <v>11.3</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="N32" s="6">
         <v>6.1</v>
@@ -2330,22 +2318,22 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B33" s="3">
         <v>0.32469999999999999</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
@@ -2361,10 +2349,10 @@
         <v>11.6</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N33" s="6">
         <v>5.8</v>
@@ -2376,22 +2364,22 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B34" s="3">
         <v>0.27100000000000002</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
@@ -2407,10 +2395,10 @@
         <v>11.9</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N34" s="6">
         <v>5.5</v>
@@ -2422,22 +2410,22 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B35" s="3">
         <v>0.26490000000000002</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
@@ -2453,10 +2441,10 @@
         <v>12.2</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N35" s="6">
         <v>5.2</v>
@@ -2468,22 +2456,22 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B36" s="3">
         <v>0.29470000000000002</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
@@ -2499,10 +2487,10 @@
         <v>12.5</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="N36" s="6">
         <v>4.9000000000000004</v>
@@ -2514,22 +2502,22 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B37" s="3">
         <v>0.37009999999999998</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
@@ -2545,10 +2533,10 @@
         <v>12.8</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N37" s="6">
         <v>4.5999999999999996</v>
@@ -2560,22 +2548,22 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B38" s="3">
         <v>0.39510000000000001</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
@@ -2591,10 +2579,10 @@
         <v>13.2</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N38" s="6">
         <v>4.2</v>
@@ -2606,22 +2594,22 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B39" s="3">
         <v>0.31019999999999998</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
@@ -2637,10 +2625,10 @@
         <v>13.6</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N39" s="6">
         <v>3.9</v>
@@ -2652,22 +2640,22 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B40" s="3">
         <v>0.3095</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
@@ -2683,10 +2671,10 @@
         <v>13.9</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N40" s="6">
         <v>3.6</v>
@@ -2698,22 +2686,22 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B41" s="3">
         <v>0.41010000000000002</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
@@ -2729,10 +2717,10 @@
         <v>14.3</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N41" s="6">
         <v>3.1</v>
@@ -2744,22 +2732,22 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B42" s="3">
         <v>0.31480000000000002</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
@@ -2775,10 +2763,10 @@
         <v>14.6</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="N42" s="6">
         <v>2.8</v>
@@ -2790,22 +2778,22 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B43" s="3">
         <v>0.29530000000000001</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
@@ -2821,10 +2809,10 @@
         <v>14.9</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N43" s="6">
         <v>2.5</v>
@@ -2836,22 +2824,22 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B44" s="3">
         <v>0.32</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
@@ -2867,10 +2855,10 @@
         <v>15.2</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="N44" s="6">
         <v>2.2000000000000002</v>
@@ -2882,22 +2870,22 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B45" s="3">
         <v>0.50449999999999995</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
@@ -2913,10 +2901,10 @@
         <v>15.7</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N45" s="6">
         <v>1.7</v>
@@ -2928,22 +2916,22 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B46" s="3">
         <v>0.33</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
@@ -2959,10 +2947,10 @@
         <v>16</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N46" s="6">
         <v>1.4</v>
@@ -2974,22 +2962,22 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B47" s="3">
         <v>0.33950000000000002</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
@@ -3005,10 +2993,10 @@
         <v>16.399999999999999</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N47" s="6">
         <v>1</v>
@@ -3020,22 +3008,22 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B48" s="3">
         <v>0.31309999999999999</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
@@ -3051,10 +3039,10 @@
         <v>16.7</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N48" s="6">
         <v>0.7</v>
@@ -3066,20 +3054,20 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B49" s="3">
         <v>0.16520000000000001</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
@@ -3095,10 +3083,10 @@
         <v>16.899999999999999</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="N49" s="6">
         <v>0.6</v>
@@ -3110,20 +3098,20 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B50" s="3">
         <v>0.2445</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
@@ -3139,10 +3127,10 @@
         <v>17.100000000000001</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="N50" s="6">
         <v>0.3</v>
@@ -3154,20 +3142,20 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B51" s="3">
         <v>0.26179999999999998</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
@@ -3183,10 +3171,10 @@
         <v>17.399999999999999</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="N51" s="6">
         <v>0.1</v>
@@ -3198,20 +3186,20 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B52" s="3">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
@@ -3227,10 +3215,10 @@
         <v>17.399999999999999</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="N52" s="6">
         <v>0</v>
@@ -3240,616 +3228,6 @@
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G54" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G59" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G61" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G62" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G63" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G66" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G67" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G73" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G74" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G75" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G76" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G77" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G78" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G79" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G80" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G81" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G82" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G83" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G84" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G85" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G86" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G87" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G88" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G89" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G90" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G91" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G92" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G93" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G94" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G95" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G97" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G98" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G99" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G100" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G101" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G102" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G103" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G104" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G105" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G106" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G107" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G108" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G109" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G110" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G111" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G112" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G113" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G114" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G115" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G116" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G117" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G118" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G119" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G120" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G121" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G122" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G123" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G124" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G125" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G126" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G127" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G128" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G129" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G130" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G131" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G132" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G133" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G134" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G135" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G136" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G137" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G138" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G139" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G140" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G141" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G142" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G143" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G144" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G145" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G146" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G147" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G148" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G149" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G150" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G151" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G152" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G153" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G154" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G155" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G156" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G157" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G158" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G159" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G160" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G161" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G162" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G163" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G164" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G165" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G166" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G167" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G168" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G169" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G170" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G171" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G172" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G173" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G174" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>